<commit_message>
added all login tests and social media tests are being prepared
</commit_message>
<xml_diff>
--- a/documentation/test_cases.xlsx
+++ b/documentation/test_cases.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="137">
   <si>
     <t>Step</t>
   </si>
@@ -186,6 +186,24 @@
   </si>
   <si>
     <t>6.3</t>
+  </si>
+  <si>
+    <t>Login with locked user</t>
+  </si>
+  <si>
+    <t>The username has been inserted</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>The password has been inserted</t>
+  </si>
+  <si>
+    <t>Login is unsuccessfull, user is not being redirected to home page. Error "Epic sadface: Sorry, this user has been locked out ".</t>
+  </si>
+  <si>
+    <t>Error "Epic sadface: Sorry, this user has been locked out ".</t>
   </si>
   <si>
     <r>
@@ -1450,6 +1468,70 @@
       </c>
       <c r="F26" s="11"/>
     </row>
+    <row r="27">
+      <c r="A27" s="13">
+        <v>7.0</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
@@ -1501,7 +1583,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3">
@@ -1509,7 +1591,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -1521,14 +1603,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F4" s="11"/>
     </row>
@@ -1537,14 +1619,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F5" s="11"/>
     </row>
@@ -1553,7 +1635,7 @@
         <v>2.0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1565,14 +1647,14 @@
         <v>22</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F7" s="11"/>
     </row>
@@ -1581,14 +1663,14 @@
         <v>23</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F8" s="11"/>
     </row>
@@ -1597,7 +1679,7 @@
         <v>3.0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1609,14 +1691,14 @@
         <v>28</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F10" s="11"/>
     </row>
@@ -1625,14 +1707,14 @@
         <v>30</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="16" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F11" s="11"/>
     </row>
@@ -1691,7 +1773,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3">
@@ -1699,7 +1781,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
@@ -1707,14 +1789,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F4" s="11"/>
     </row>
@@ -1723,14 +1805,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F5" s="11"/>
     </row>
@@ -1739,14 +1821,14 @@
         <v>18</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="10" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F6" s="11"/>
     </row>
@@ -1755,7 +1837,7 @@
         <v>2.0</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
@@ -1763,14 +1845,14 @@
         <v>22</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F8" s="11"/>
     </row>
@@ -1779,14 +1861,14 @@
         <v>23</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F9" s="11"/>
     </row>
@@ -1795,14 +1877,14 @@
         <v>25</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F10" s="11"/>
     </row>
@@ -1811,7 +1893,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12">
@@ -1819,14 +1901,14 @@
         <v>28</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F12" s="11"/>
     </row>
@@ -1835,14 +1917,14 @@
         <v>30</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F13" s="11"/>
     </row>
@@ -1851,14 +1933,14 @@
         <v>31</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="10" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F14" s="11"/>
     </row>
@@ -1867,7 +1949,7 @@
         <v>4.0</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
@@ -1875,14 +1957,14 @@
         <v>33</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F16" s="11"/>
     </row>
@@ -1891,14 +1973,14 @@
         <v>35</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="21" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F17" s="11"/>
     </row>
@@ -1907,14 +1989,14 @@
         <v>37</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="10" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="F18" s="11"/>
     </row>
@@ -1971,7 +2053,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3">
@@ -1979,7 +2061,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
@@ -1987,14 +2069,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F4" s="10"/>
     </row>
@@ -2003,14 +2085,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F5" s="10"/>
     </row>
@@ -2019,7 +2101,7 @@
         <v>2.0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
@@ -2027,14 +2109,14 @@
         <v>22</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F7" s="10"/>
     </row>
@@ -2043,14 +2125,14 @@
         <v>23</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -2059,7 +2141,7 @@
         <v>3.0</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
@@ -2067,14 +2149,14 @@
         <v>28</v>
       </c>
       <c r="B10" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F10" s="10"/>
     </row>
@@ -2083,14 +2165,14 @@
         <v>30</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F11" s="10"/>
     </row>
@@ -2147,7 +2229,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
@@ -2155,7 +2237,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4">
@@ -2163,14 +2245,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F4" s="10"/>
     </row>
@@ -2179,14 +2261,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F5" s="10"/>
     </row>
@@ -2195,14 +2277,14 @@
         <v>18</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F6" s="10"/>
     </row>
@@ -2211,7 +2293,7 @@
         <v>2.0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
@@ -2219,14 +2301,14 @@
         <v>9</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -2235,14 +2317,14 @@
         <v>13</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F9" s="10"/>
     </row>
@@ -2251,14 +2333,14 @@
         <v>18</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F10" s="10"/>
     </row>
@@ -2267,7 +2349,7 @@
         <v>3.0</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12">
@@ -2275,14 +2357,14 @@
         <v>9</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F12" s="10"/>
     </row>
@@ -2291,14 +2373,14 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F13" s="10"/>
     </row>
@@ -2307,14 +2389,14 @@
         <v>18</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F14" s="10"/>
     </row>
@@ -2371,7 +2453,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -2379,7 +2461,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4">
@@ -2387,14 +2469,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F4" s="10"/>
     </row>
@@ -2403,14 +2485,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F5" s="10"/>
     </row>
@@ -2419,7 +2501,7 @@
         <v>2.0</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7">
@@ -2427,14 +2509,14 @@
         <v>22</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F7" s="10"/>
     </row>
@@ -2443,14 +2525,14 @@
         <v>23</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -2506,7 +2588,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
@@ -2514,7 +2596,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4">
@@ -2522,14 +2604,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F4" s="10"/>
     </row>
@@ -2538,14 +2620,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F5" s="10"/>
     </row>
@@ -2554,14 +2636,14 @@
         <v>44929.0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F6" s="10"/>
     </row>
@@ -2570,14 +2652,14 @@
         <v>44930.0</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F7" s="10"/>
     </row>
@@ -2634,7 +2716,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3">
@@ -2642,7 +2724,7 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4">
@@ -2650,14 +2732,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F4" s="10"/>
     </row>
@@ -2666,14 +2748,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F5" s="10"/>
     </row>
@@ -2682,14 +2764,14 @@
         <v>44929.0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="F6" s="10"/>
     </row>
@@ -2698,14 +2780,14 @@
         <v>44930.0</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="F7" s="10"/>
     </row>
@@ -2714,14 +2796,14 @@
         <v>44931.0</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="16" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -2730,16 +2812,16 @@
         <v>44932.0</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="F9" s="10"/>
     </row>
@@ -2748,16 +2830,16 @@
         <v>44933.0</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F10" s="10"/>
     </row>
@@ -2766,16 +2848,16 @@
         <v>44934.0</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F11" s="10"/>
     </row>
@@ -2784,14 +2866,14 @@
         <v>44935.0</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="18" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="F12" s="10"/>
     </row>
@@ -2800,14 +2882,14 @@
         <v>44936.0</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="F13" s="10"/>
     </row>
@@ -2816,14 +2898,14 @@
         <v>44937.0</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F14" s="10"/>
     </row>

</xml_diff>